<commit_message>
species added to mixing models,
species models
concentration dependency added
run on very long
</commit_message>
<xml_diff>
--- a/data/Phytoplankton Calculation from Fry 2002.xlsx
+++ b/data/Phytoplankton Calculation from Fry 2002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coastal54-my.sharepoint.com/personal/rrezek_coastal_edu/Documents/Rezek Lab/Student Files/Grace Kahmann/Mixng model stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17035\Desktop\New GitHub\Brown-vs-Green\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{EE748346-1294-4F4B-B54C-C1E072A51EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F2C5DFA-E8F2-4A70-94C2-B07D474A6358}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396B5287-CCC4-4DF0-8719-0B093009521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="29325" yWindow="1830" windowWidth="23340" windowHeight="14070" xr2:uid="{0585427B-9D6B-488F-A954-7282565750D8}"/>
+    <workbookView xWindow="46575" yWindow="1185" windowWidth="27975" windowHeight="21000" xr2:uid="{0585427B-9D6B-488F-A954-7282565750D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,21 +463,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDB673B-B810-43CD-A34F-AF38DA79FA71}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -511,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -536,7 +536,7 @@
         <v>0.83666002653407512</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -547,12 +547,12 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>22</v>
@@ -567,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -587,12 +587,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>22</v>
@@ -615,7 +615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -636,17 +636,17 @@
         <v>1.1313708498984771</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>31</v>
       </c>
@@ -668,7 +668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -686,7 +686,7 @@
         <v>3.0405591591021572</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -697,7 +697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>31</v>
       </c>
@@ -705,7 +705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
@@ -720,12 +720,12 @@
         <v>2.1213203435596424</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2</v>
       </c>
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>31</v>
       </c>
@@ -753,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1.3279056191361454</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -786,17 +786,17 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>2</v>
       </c>
@@ -810,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>6</v>
       </c>
@@ -818,7 +818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -836,7 +836,7 @@
         <v>0.9192388155425123</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>20</v>
       </c>
@@ -847,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>6</v>
       </c>
@@ -855,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -873,12 +873,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>2</v>
       </c>
@@ -886,7 +886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>6</v>
       </c>
@@ -906,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
         <v>1.85831464863551</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>